<commit_message>
4th submit with profit loss features added
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>submit</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>random foreset, in modifed 3in1 data set (convert train to bonus feature like dataset then agg), train on 1-34, valid on 41 - 43 (.87)</t>
+  </si>
+  <si>
+    <t>4_201115_0909_rf_with_3in1_added_profitloss_relatd_features</t>
+  </si>
+  <si>
+    <t>0.57+</t>
+  </si>
+  <si>
+    <t>random foreset, in modifed 3in1 data set (new profit loss related features), train on 1-34, valid on 41 - 43 (.88)</t>
   </si>
 </sst>
 </file>
@@ -94,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -106,13 +117,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,6 +508,17 @@
       </c>
       <c r="C4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5th - suprisingly shitty submit with only .53 score
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>submit</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>random foreset, in modifed 3in1 data set (new profit loss related features), train on 1-34, valid on 41 - 43 (.88)</t>
+  </si>
+  <si>
+    <t>5_201115_2117_rf_with_3in1_corrected_train_and_valid</t>
+  </si>
+  <si>
+    <t>random foreset, in 3in1 data set, corrected train and valid set. Train (.84), valid (.82)</t>
   </si>
 </sst>
 </file>
@@ -455,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -519,6 +525,17 @@
       </c>
       <c r="C5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0.53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6th rf with 3in1 with not valid set
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>submit</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>random foreset, in 3in1 data set, corrected train and valid set. Train (.84), valid (.82)</t>
+  </si>
+  <si>
+    <t>6_211115_1297_rf_with_3in1_no_valid</t>
+  </si>
+  <si>
+    <t>random forest, in 3in1 data set, with no valid set</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -538,6 +544,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>0.56464999999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
7th: 7 xgboost on 3in1 with valid1 and valid1
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>submit</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>random forest, in 3in1 data set, with no valid set</t>
+  </si>
+  <si>
+    <t>7_281115_1041_7_xgboost_with_3in1_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 xgboost, in 3in1 data set, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -555,6 +561,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
8th: 8 xgboost on 3in1 with feature preprocessed with 2 valid sets
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>submit</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>ensembled 7 xgboost, in 3in1 data set, with 2 valid sets</t>
+  </si>
+  <si>
+    <t>8_281115_1914_7_xgboost_with_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 xgboost, in 3in1 data set with features preprocessed, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -121,8 +127,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -135,15 +143,17 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -572,6 +582,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>0.622</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
9th 50xgboost on non overlapping 3in1 with preprocessed and with 2 valid sets
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>submit</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>ensembled 7 xgboost, in 3in1 data set with features preprocessed, with 2 valid sets</t>
+  </si>
+  <si>
+    <t>9_291115_0944_50_xgboost_with_non_overlap_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 50 xgboost, in non_overlapping 3in1 data set with features preprocessed, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -127,8 +133,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -143,17 +151,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,6 +603,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
7 xgboost with random 3in1 with preprocessed with valid1 and valid2
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>submit</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>ensembled 50 xgboost, in non_overlapping 3in1 data set with features preprocessed, with 2 valid sets</t>
+  </si>
+  <si>
+    <t>10_291115_2231_7_xgboost_with_random_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 xgboost, in random 3in1 data set with features preprocessed, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -614,6 +620,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>0.62914999999999999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
15th: 7 tree xgboost binary logits and 1 linear xgboost binary logits on random 3in1 with preprocessed with valid1 and valid2
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>submit</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>ensembled 7 tree xgboost and 1 lienar xgboost on random combined 3in1 data set with features preprocessed, with 2 valid sets</t>
+  </si>
+  <si>
+    <t>14_011215_0718_7_xgboost_binary_logits_with_random_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 tree xgboost binary logits on random combined 3in1 data set with features preprocessed, with 2 valid sets</t>
+  </si>
+  <si>
+    <t>15_011215_0818_7_tree_xgboost_binary_logits_and_1_linear_xgboost_binary_logits_with_random_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 tree xgboost binary logits and 1 linear xgboost binary logits on random combined 3in1 data set with features preprocessed, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -157,8 +169,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,7 +199,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -194,6 +210,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -204,6 +222,8 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -698,6 +718,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>0.63185999999999998</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>0.63527999999999996</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
more random 3in1 failed and doing feature selection
</commit_message>
<xml_diff>
--- a/submit/summary_submit_and_score.xlsx
+++ b/submit/summary_submit_and_score.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>submit</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>lasso lr on more random 3in1, and xgboost on less randome 3in1</t>
+  </si>
+  <si>
+    <t>18_021215_2150_7_xgboost_binary_logits_with_more_random_3in1_preprocess_valid1_valid2_</t>
+  </si>
+  <si>
+    <t>ensembled 7 tree xgboost binary logits on more random combined 3in1 data set with features preprocessed, with 2 valid sets</t>
   </si>
 </sst>
 </file>
@@ -181,8 +187,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -211,7 +219,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -224,6 +232,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -236,6 +245,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -774,6 +784,17 @@
         <v>37</v>
       </c>
     </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>0.63119999999999998</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>